<commit_message>
Exportacao automatica xlsx -> json em gulpfile('gulp create-json')
</commit_message>
<xml_diff>
--- a/monitoramento.xlsx
+++ b/monitoramento.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\teste-xlsx\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38370" windowHeight="10185"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -47,9 +46,6 @@
     <t>Morbi ipsum nunc, aliquam ac dolor hendrerit, posuere viverra lorem. Orci varius natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Vestibulum sed mauris urna. Integer volutpat elementum dui in suscipit. Suspendisse efficitur, metus tristique pharetra varius, metus massa imperdiet lectus, nec finibus orci nisl vitae ex. Pellentesque finibus et justo a posuere. Ut placerat quam purus, iaculis consequat nisi porta eget. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos</t>
   </si>
   <si>
-    <t>Phasellus rutrum nibh dolor, pellentesque malesuada felis pharetra semper. Maecenas porta, orci ac rhoncus mollis, velit magna pulvinar erat, eget gravida massa massa nec libero. Vivamus iaculis, odio et porttitor sollicitudin, velit augue ultricies risus, eu eleifend purus est in neque. Pellentesque et nisl justo. Proin dictum ullamcorper justo a commodo. Praesent consectetur est ut risus tincidunt consectetur. Interdum et malesuada fames ac ante ipsum primis in faucibus. Nunc et facilisis dui. Sed felis purus, maximus quis interdum et, sodales non diam. Integer fringilla tellus nisl, ac vehicula felis volutpat bibendum.</t>
-  </si>
-  <si>
     <t>texto_longo</t>
   </si>
   <si>
@@ -69,13 +65,16 @@
   </si>
   <si>
     <t>datas</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,6 +128,31 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="info"/>
+      <sheetName val="ETAPAS_STATUS"/>
+      <sheetName val="Atividades"/>
+      <sheetName val="legenda_cores"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="8">
+          <cell r="V8" t="str">
+            <v>Aprovado</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
@@ -172,7 +196,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -207,7 +231,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -384,29 +408,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.25" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -414,19 +438,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -434,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1">
         <v>20</v>
@@ -446,7 +470,7 @@
         <v>43194</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -454,7 +478,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1">
         <v>200</v>
@@ -466,7 +490,7 @@
         <v>43163</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -474,13 +498,14 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1">
         <v>2000</v>
       </c>
-      <c r="E4" t="s">
-        <v>7</v>
+      <c r="E4" t="str">
+        <f>[1]info!$V$8</f>
+        <v>Aprovado</v>
       </c>
       <c r="F4" s="2">
         <v>43135</v>
@@ -490,4 +515,22 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ajuste de ambiente de desenvolvimento com tema gestaourbanasp
</commit_message>
<xml_diff>
--- a/monitoramento.xlsx
+++ b/monitoramento.xlsx
@@ -10,9 +10,6 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
     <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -23,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -31,43 +28,61 @@
     <t>nome</t>
   </si>
   <si>
+    <t>projeto 2</t>
+  </si>
+  <si>
+    <t>projeto 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Fusce mauris eros, pretium id rhoncus sit amet, sollicitudin at est. Vestibulum iaculis blandit nunc, in euismod lorem semper nec. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam eu ipsum condimentum, rutrum velit et, malesuada augue. Fusce in lacus ut risus molestie ornare. Aenean ultricies fermentum nibh, sagittis vestibulum nisi convallis eu. Nunc eget metus arcu. </t>
+  </si>
+  <si>
+    <t>Morbi ipsum nunc, aliquam ac dolor hendrerit, posuere viverra lorem. Orci varius natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Vestibulum sed mauris urna. Integer volutpat elementum dui in suscipit. Suspendisse efficitur, metus tristique pharetra varius, metus massa imperdiet lectus, nec finibus orci nisl vitae ex. Pellentesque finibus et justo a posuere. Ut placerat quam purus, iaculis consequat nisi porta eget. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos</t>
+  </si>
+  <si>
+    <t>texto_longo</t>
+  </si>
+  <si>
+    <t>valor_numerico</t>
+  </si>
+  <si>
+    <t>categorias</t>
+  </si>
+  <si>
+    <t>categoria 1</t>
+  </si>
+  <si>
+    <t>categoria 2</t>
+  </si>
+  <si>
+    <t>categoria 3</t>
+  </si>
+  <si>
+    <t>datas</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
     <t>projeto 1</t>
   </si>
   <si>
-    <t>projeto 2</t>
-  </si>
-  <si>
-    <t>projeto 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Fusce mauris eros, pretium id rhoncus sit amet, sollicitudin at est. Vestibulum iaculis blandit nunc, in euismod lorem semper nec. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam eu ipsum condimentum, rutrum velit et, malesuada augue. Fusce in lacus ut risus molestie ornare. Aenean ultricies fermentum nibh, sagittis vestibulum nisi convallis eu. Nunc eget metus arcu. </t>
-  </si>
-  <si>
-    <t>Morbi ipsum nunc, aliquam ac dolor hendrerit, posuere viverra lorem. Orci varius natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus. Vestibulum sed mauris urna. Integer volutpat elementum dui in suscipit. Suspendisse efficitur, metus tristique pharetra varius, metus massa imperdiet lectus, nec finibus orci nisl vitae ex. Pellentesque finibus et justo a posuere. Ut placerat quam purus, iaculis consequat nisi porta eget. Class aptent taciti sociosqu ad litora torquent per conubia nostra, per inceptos himenaeos</t>
-  </si>
-  <si>
-    <t>texto_longo</t>
-  </si>
-  <si>
-    <t>valor_numerico</t>
-  </si>
-  <si>
-    <t>categorias</t>
-  </si>
-  <si>
-    <t>categoria 1</t>
-  </si>
-  <si>
-    <t>categoria 2</t>
-  </si>
-  <si>
-    <t>categoria 3</t>
-  </si>
-  <si>
-    <t>datas</t>
-  </si>
-  <si>
-    <t>asd</t>
+    <t>Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
+  </si>
+  <si>
+    <t>kml</t>
+  </si>
+  <si>
+    <t>piu-arco-jurubatuba_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-arco-pinheiros_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-arco-tiete_2018-04.kml</t>
+  </si>
+  <si>
+    <t>ponto_central</t>
   </si>
 </sst>
 </file>
@@ -103,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -111,6 +126,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -126,31 +142,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="info"/>
-      <sheetName val="ETAPAS_STATUS"/>
-      <sheetName val="Atividades"/>
-      <sheetName val="legenda_cores"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="8">
-          <cell r="V8" t="str">
-            <v>Aprovado</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,21 +407,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.25" customWidth="1"/>
-    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,77 +431,91 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1">
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2">
         <v>43194</v>
       </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1">
         <v>200</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2">
         <v>43163</v>
       </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <v>2000</v>
       </c>
-      <c r="E4" t="str">
-        <f>[1]info!$V$8</f>
-        <v>Aprovado</v>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="F4" s="2">
         <v>43135</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +534,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Comeco CSS e js do sumario
</commit_message>
<xml_diff>
--- a/monitoramento.xlsx
+++ b/monitoramento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -83,14 +83,88 @@
   </si>
   <si>
     <t>ponto_central</t>
+  </si>
+  <si>
+    <t>projeto 4</t>
+  </si>
+  <si>
+    <t>categoria 4</t>
+  </si>
+  <si>
+    <t>projeto 5</t>
+  </si>
+  <si>
+    <t>categoria 5</t>
+  </si>
+  <si>
+    <t>projeto 6</t>
+  </si>
+  <si>
+    <t>categoria 6</t>
+  </si>
+  <si>
+    <t>projeto 7</t>
+  </si>
+  <si>
+    <t>categoria 7</t>
+  </si>
+  <si>
+    <t>projeto 8</t>
+  </si>
+  <si>
+    <t>categoria 8</t>
+  </si>
+  <si>
+    <t>projeto 9</t>
+  </si>
+  <si>
+    <t>categoria 9</t>
+  </si>
+  <si>
+    <t>projeto 10</t>
+  </si>
+  <si>
+    <t>categoria 10</t>
+  </si>
+  <si>
+    <t>projeto 11</t>
+  </si>
+  <si>
+    <t>categoria 11</t>
+  </si>
+  <si>
+    <t>projeto 12</t>
+  </si>
+  <si>
+    <t>categoria 12</t>
+  </si>
+  <si>
+    <t>subetapa</t>
+  </si>
+  <si>
+    <t>natureza</t>
+  </si>
+  <si>
+    <t>publico</t>
+  </si>
+  <si>
+    <t>privado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -118,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -127,6 +201,7 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +474,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -407,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -423,7 +498,7 @@
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,8 +523,14 @@
       <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -471,8 +552,14 @@
       <c r="G2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="4">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -494,8 +581,14 @@
       <c r="G3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="4">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -516,6 +609,252 @@
       </c>
       <c r="G4" t="s">
         <v>19</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2001</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43136</v>
+      </c>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2002</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2">
+        <v>43137</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2003</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43138</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2004</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2">
+        <v>43139</v>
+      </c>
+      <c r="G8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2005</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43140</v>
+      </c>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2006</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43141</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2007</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="2">
+        <v>43142</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="2">
+        <v>43143</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2009</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="2">
+        <v>43144</v>
+      </c>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="4">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterar gulpfile para puxar monitoramento.js em modo watch
</commit_message>
<xml_diff>
--- a/monitoramento.xlsx
+++ b/monitoramento.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>id</t>
   </si>
@@ -28,12 +28,6 @@
     <t>nome</t>
   </si>
   <si>
-    <t>projeto 2</t>
-  </si>
-  <si>
-    <t>projeto 3</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Fusce mauris eros, pretium id rhoncus sit amet, sollicitudin at est. Vestibulum iaculis blandit nunc, in euismod lorem semper nec. Vestibulum ante ipsum primis in faucibus orci luctus et ultrices posuere cubilia Curae; Aliquam eu ipsum condimentum, rutrum velit et, malesuada augue. Fusce in lacus ut risus molestie ornare. Aenean ultricies fermentum nibh, sagittis vestibulum nisi convallis eu. Nunc eget metus arcu. </t>
   </si>
   <si>
@@ -64,9 +58,6 @@
     <t>asd</t>
   </si>
   <si>
-    <t>projeto 1</t>
-  </si>
-  <si>
     <t>Lorem ipsum dolor sit amet, consectetur adipisicing elit, sed do eiusmod tempor incididunt ut labore et dolore magna aliqua. Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut aliquip ex ea commodo consequat. Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore eu fugiat nulla pariatur. Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia deserunt mollit anim id est laborum.</t>
   </si>
   <si>
@@ -83,6 +74,96 @@
   </si>
   <si>
     <t>ponto_central</t>
+  </si>
+  <si>
+    <t>piu-anhembi_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-area-central_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-nacoes-unidas_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-nesp_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-pacaembu_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-rio-branco_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-terminais-pilotos_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-vila-leopoldina_2018-04.kml</t>
+  </si>
+  <si>
+    <t>piu-vila-olimpia_2018-04.kml</t>
+  </si>
+  <si>
+    <t>categoria 4</t>
+  </si>
+  <si>
+    <t>categoria 5</t>
+  </si>
+  <si>
+    <t>categoria 6</t>
+  </si>
+  <si>
+    <t>categoria 7</t>
+  </si>
+  <si>
+    <t>categoria 8</t>
+  </si>
+  <si>
+    <t>categoria 9</t>
+  </si>
+  <si>
+    <t>categoria 10</t>
+  </si>
+  <si>
+    <t>categoria 11</t>
+  </si>
+  <si>
+    <t>categoria 12</t>
+  </si>
+  <si>
+    <t>anhembi</t>
+  </si>
+  <si>
+    <t>jurubatuba</t>
+  </si>
+  <si>
+    <t>pinheiros</t>
+  </si>
+  <si>
+    <t>tiete</t>
+  </si>
+  <si>
+    <t>area-central</t>
+  </si>
+  <si>
+    <t>nacoes-unidas</t>
+  </si>
+  <si>
+    <t>nesp</t>
+  </si>
+  <si>
+    <t>pacaembu</t>
+  </si>
+  <si>
+    <t>rio-branco</t>
+  </si>
+  <si>
+    <t>terminais-piloto</t>
+  </si>
+  <si>
+    <t>vila-leopoldina</t>
+  </si>
+  <si>
+    <t>vila-olimpia</t>
   </si>
 </sst>
 </file>
@@ -399,7 +480,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -407,19 +488,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.28515625" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -431,22 +513,22 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -454,22 +536,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>20</v>
+        <v>123</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="2">
         <v>43194</v>
       </c>
       <c r="G2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -477,22 +559,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>200</v>
+        <v>456</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2">
         <v>43163</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -500,22 +582,229 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1">
+        <v>123</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1">
+        <v>456</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1">
+        <v>123</v>
+      </c>
+      <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F6" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="1">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8564</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1">
+        <v>123</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1">
+        <v>546</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1">
+        <v>98</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="D4" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2">
-        <v>43135</v>
-      </c>
-      <c r="G4" t="s">
-        <v>19</v>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5461</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1">
+        <v>123654</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="2">
+        <v>43135</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -528,13 +817,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Altera gulpfile. Nodejs monta monitoramento.js. Frontend desacoplado do excel tambem em desenvolvimento
</commit_message>
<xml_diff>
--- a/monitoramento.xlsx
+++ b/monitoramento.xlsx
@@ -142,28 +142,28 @@
     <t>tiete</t>
   </si>
   <si>
-    <t>area-central</t>
-  </si>
-  <si>
-    <t>nacoes-unidas</t>
-  </si>
-  <si>
     <t>nesp</t>
   </si>
   <si>
     <t>pacaembu</t>
   </si>
   <si>
-    <t>rio-branco</t>
-  </si>
-  <si>
-    <t>terminais-piloto</t>
-  </si>
-  <si>
-    <t>vila-leopoldina</t>
-  </si>
-  <si>
-    <t>vila-olimpia</t>
+    <t>area_central</t>
+  </si>
+  <si>
+    <t>nacoes_unidas</t>
+  </si>
+  <si>
+    <t>rio_branco</t>
+  </si>
+  <si>
+    <t>terminais_piloto</t>
+  </si>
+  <si>
+    <t>vila_leopoldina</t>
+  </si>
+  <si>
+    <t>vila_olimpia</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -628,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>28</v>
@@ -651,7 +651,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>29</v>
@@ -674,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>30</v>
@@ -697,7 +697,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>

</xml_diff>